<commit_message>
AutoCommit_16 октября 2023 г. 14:01:13_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -518,10 +518,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -698,6 +698,9 @@
       <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -709,6 +712,9 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -759,6 +765,12 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -894,6 +906,9 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="G26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_17 октября 2023 г. 9:12:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -518,7 +518,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
@@ -615,6 +615,9 @@
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -668,6 +671,9 @@
         <v>5</v>
       </c>
       <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
@@ -694,7 +700,9 @@
         <v>30</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
@@ -733,6 +741,9 @@
       <c r="G14" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H14" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -764,7 +775,9 @@
         <v>30</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>30</v>
       </c>
@@ -854,6 +867,9 @@
       <c r="G22" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H22" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -925,8 +941,13 @@
       <c r="D27" s="2">
         <v>5</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -945,6 +966,9 @@
       <c r="G28" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -958,8 +982,11 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="H29" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_17 октября 2023 г. 9:17:39_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Дз6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">и </t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +194,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -211,6 +225,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -518,10 +535,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -612,6 +629,9 @@
         <v>5</v>
       </c>
       <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
@@ -652,8 +672,16 @@
         <v>30</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -677,6 +705,9 @@
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H10" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -701,6 +732,9 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -755,8 +789,13 @@
       <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>30</v>
       </c>
@@ -797,6 +836,9 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>30</v>
       </c>
@@ -864,6 +906,9 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>30</v>
       </c>
@@ -894,6 +939,9 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G24" s="2" t="s">
         <v>30</v>
       </c>
@@ -944,6 +992,9 @@
       <c r="E27" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="F27" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G27" s="2" t="s">
         <v>30</v>
       </c>
@@ -963,6 +1014,9 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G28" s="2" t="s">
         <v>30</v>
       </c>
@@ -982,6 +1036,9 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="H29" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_17 октября 2023 г. 9:19:24_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -223,11 +223,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -535,10 +535,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -549,29 +549,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -628,7 +628,9 @@
       <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
@@ -705,7 +707,7 @@
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -937,7 +939,9 @@
       <c r="C24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
         <v>30</v>
@@ -969,6 +973,9 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G26" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_17 октября 2023 г. 9:21:20_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -535,10 +535,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1019,9 @@
       <c r="C28" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
AutoCommit_17 октября 2023 г. 9:54:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -535,10 +535,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,9 @@
       <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
AutoCommit_24 октября 2023 г. 10:01:29_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1185,15 +1185,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
AutoCommit_27 октября 2023 г. 13:02:28_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -930,7 +930,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -953,8 +953,19 @@
       <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">

</xml_diff>

<commit_message>
AutoCommit_27 октября 2023 г. 13:03:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -111,9 +111,6 @@
     <t>ок</t>
   </si>
   <si>
-    <t>Камилецкий</t>
-  </si>
-  <si>
     <t>Дз2</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>ко</t>
+  </si>
+  <si>
+    <t>Каменецкий</t>
   </si>
 </sst>
 </file>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -591,22 +591,22 @@
         <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1043,7 +1043,7 @@
         <v>29</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1198,9 +1198,18 @@
     </row>
     <row r="33" spans="2:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G33" s="2" t="s">

</xml_diff>

<commit_message>
AutoCommit_7 ноября 2023 г. 9:21:38_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -958,11 +958,27 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">

</xml_diff>

<commit_message>
AutoCommit_7 ноября 2023 г. 9:23:33_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 14:24:20_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -547,10 +547,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -793,6 +793,9 @@
       <c r="I12" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -860,6 +863,9 @@
         <v>29</v>
       </c>
       <c r="I15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_22 ноября 2023 г. 9:32:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -136,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -159,13 +159,40 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -215,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -236,11 +263,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -548,10 +585,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -562,29 +599,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -622,7 +659,7 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="11">
         <v>5</v>
       </c>
       <c r="D5" s="2"/>
@@ -653,10 +690,10 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="11">
+        <v>5</v>
+      </c>
+      <c r="D6" s="11">
         <v>5</v>
       </c>
       <c r="E6" s="2">
@@ -689,7 +726,7 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="11">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
@@ -735,10 +772,10 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="11">
+        <v>5</v>
+      </c>
+      <c r="D9" s="11">
         <v>5</v>
       </c>
       <c r="E9" s="2">
@@ -771,10 +808,10 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="11">
+        <v>5</v>
+      </c>
+      <c r="D10" s="11">
         <v>5</v>
       </c>
       <c r="E10" s="2">
@@ -822,10 +859,10 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="11">
+        <v>5</v>
+      </c>
+      <c r="D12" s="11">
         <v>5</v>
       </c>
       <c r="E12" s="2">
@@ -852,24 +889,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:23" s="14" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
         <v>9</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="H13" s="2">
-        <v>5</v>
-      </c>
-      <c r="K13" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M13">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="H13" s="13">
+        <v>5</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M13" s="14">
         <v>2</v>
       </c>
     </row>
@@ -880,10 +917,10 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="11">
+        <v>5</v>
+      </c>
+      <c r="D14" s="11">
         <v>5</v>
       </c>
       <c r="E14" s="2">
@@ -913,10 +950,10 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="11">
+        <v>5</v>
+      </c>
+      <c r="D15" s="11">
         <v>5</v>
       </c>
       <c r="E15" s="2">
@@ -950,10 +987,10 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="11">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11">
         <v>5</v>
       </c>
       <c r="E16" s="2">
@@ -986,10 +1023,10 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="11">
+        <v>5</v>
+      </c>
+      <c r="D17" s="11">
         <v>5</v>
       </c>
       <c r="E17" s="2">
@@ -1040,7 +1077,7 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="11">
         <v>5</v>
       </c>
       <c r="D19" s="2"/>
@@ -1051,7 +1088,7 @@
       <c r="H19" s="2">
         <v>5</v>
       </c>
-      <c r="I19" s="10"/>
+      <c r="I19" s="8"/>
       <c r="K19" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1067,10 +1104,10 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="11">
+        <v>5</v>
+      </c>
+      <c r="D20" s="11">
         <v>5</v>
       </c>
       <c r="E20" s="2">
@@ -1103,10 +1140,10 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="11">
+        <v>5</v>
+      </c>
+      <c r="D21" s="11">
         <v>5</v>
       </c>
       <c r="E21" s="2"/>
@@ -1135,10 +1172,10 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="11">
+        <v>5</v>
+      </c>
+      <c r="D22" s="11">
         <v>5</v>
       </c>
       <c r="E22" s="2">
@@ -1171,10 +1208,10 @@
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="11">
+        <v>5</v>
+      </c>
+      <c r="D23" s="11">
         <v>5</v>
       </c>
       <c r="E23" s="2">
@@ -1204,10 +1241,10 @@
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="11">
+        <v>5</v>
+      </c>
+      <c r="D24" s="11">
         <v>5</v>
       </c>
       <c r="E24" s="2"/>
@@ -1235,7 +1272,7 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="11">
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
@@ -1263,10 +1300,10 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="11">
+        <v>5</v>
+      </c>
+      <c r="D26" s="11">
         <v>5</v>
       </c>
       <c r="E26" s="2">
@@ -1299,10 +1336,10 @@
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="11">
+        <v>5</v>
+      </c>
+      <c r="D27" s="11">
         <v>5</v>
       </c>
       <c r="E27" s="2">
@@ -1335,10 +1372,10 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="C28" s="11">
+        <v>5</v>
+      </c>
+      <c r="D28" s="11">
         <v>5</v>
       </c>
       <c r="E28" s="2">
@@ -1371,7 +1408,7 @@
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="11">
         <v>5</v>
       </c>
       <c r="D29" s="2"/>
@@ -1419,7 +1456,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2">
+      <c r="D31" s="11">
         <v>5</v>
       </c>
       <c r="E31" s="2">
@@ -1498,5 +1535,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_22 ноября 2023 г. 10:21:23_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -242,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -266,8 +266,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -278,6 +276,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -585,10 +586,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -599,29 +600,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -659,14 +660,14 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>5</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="9">
+        <v>5</v>
+      </c>
+      <c r="F5" s="15">
         <v>5</v>
       </c>
       <c r="G5" s="2">
@@ -690,16 +691,16 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>5</v>
+      </c>
+      <c r="F6" s="9">
         <v>5</v>
       </c>
       <c r="G6" s="2">
@@ -726,14 +727,14 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="9">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9">
         <v>5</v>
       </c>
       <c r="G7" s="2">
@@ -772,16 +773,16 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11">
-        <v>5</v>
-      </c>
-      <c r="D9" s="11">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="C9" s="9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9">
         <v>5</v>
       </c>
       <c r="G9" s="2">
@@ -808,16 +809,16 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11">
-        <v>5</v>
-      </c>
-      <c r="D10" s="11">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="C10" s="9">
+        <v>5</v>
+      </c>
+      <c r="D10" s="9">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9">
         <v>5</v>
       </c>
       <c r="G10" s="2">
@@ -859,16 +860,16 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="11">
-        <v>5</v>
-      </c>
-      <c r="D12" s="11">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="C12" s="9">
+        <v>5</v>
+      </c>
+      <c r="D12" s="9">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9">
+        <v>5</v>
+      </c>
+      <c r="F12" s="9">
         <v>5</v>
       </c>
       <c r="G12" s="2">
@@ -889,24 +890,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="14" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+    <row r="13" spans="1:23" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <v>9</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="H13" s="13">
-        <v>5</v>
-      </c>
-      <c r="K13" s="14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M13" s="14">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="H13" s="11">
+        <v>5</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M13" s="12">
         <v>2</v>
       </c>
     </row>
@@ -917,16 +918,16 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="11">
-        <v>5</v>
-      </c>
-      <c r="D14" s="11">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="C14" s="9">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5</v>
+      </c>
+      <c r="F14" s="9">
         <v>5</v>
       </c>
       <c r="G14" s="2">
@@ -950,16 +951,16 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="11">
-        <v>5</v>
-      </c>
-      <c r="D15" s="11">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="C15" s="9">
+        <v>5</v>
+      </c>
+      <c r="D15" s="9">
+        <v>5</v>
+      </c>
+      <c r="E15" s="9">
+        <v>5</v>
+      </c>
+      <c r="F15" s="9">
         <v>5</v>
       </c>
       <c r="G15" s="2">
@@ -987,16 +988,16 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="11">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="C16" s="9">
+        <v>5</v>
+      </c>
+      <c r="D16" s="9">
+        <v>5</v>
+      </c>
+      <c r="E16" s="9">
+        <v>5</v>
+      </c>
+      <c r="F16" s="9">
         <v>5</v>
       </c>
       <c r="G16" s="2">
@@ -1023,16 +1024,16 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="11">
-        <v>5</v>
-      </c>
-      <c r="D17" s="11">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="C17" s="9">
+        <v>5</v>
+      </c>
+      <c r="D17" s="9">
+        <v>5</v>
+      </c>
+      <c r="E17" s="9">
+        <v>5</v>
+      </c>
+      <c r="F17" s="9">
         <v>5</v>
       </c>
       <c r="G17" s="2">
@@ -1077,7 +1078,7 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="9">
         <v>5</v>
       </c>
       <c r="D19" s="2"/>
@@ -1104,16 +1105,16 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="11">
-        <v>5</v>
-      </c>
-      <c r="D20" s="11">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="C20" s="9">
+        <v>5</v>
+      </c>
+      <c r="D20" s="9">
+        <v>5</v>
+      </c>
+      <c r="E20" s="9">
+        <v>5</v>
+      </c>
+      <c r="F20" s="9">
         <v>5</v>
       </c>
       <c r="G20" s="2">
@@ -1140,14 +1141,14 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="11">
-        <v>5</v>
-      </c>
-      <c r="D21" s="11">
+      <c r="C21" s="9">
+        <v>5</v>
+      </c>
+      <c r="D21" s="9">
         <v>5</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="2">
+      <c r="F21" s="9">
         <v>5</v>
       </c>
       <c r="G21" s="2">
@@ -1172,16 +1173,16 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="11">
-        <v>5</v>
-      </c>
-      <c r="D22" s="11">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="C22" s="9">
+        <v>5</v>
+      </c>
+      <c r="D22" s="9">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9">
+        <v>5</v>
+      </c>
+      <c r="F22" s="9">
         <v>5</v>
       </c>
       <c r="G22" s="2">
@@ -1208,16 +1209,16 @@
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="11">
-        <v>5</v>
-      </c>
-      <c r="D23" s="11">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="C23" s="9">
+        <v>5</v>
+      </c>
+      <c r="D23" s="9">
+        <v>5</v>
+      </c>
+      <c r="E23" s="9">
+        <v>5</v>
+      </c>
+      <c r="F23" s="9">
         <v>5</v>
       </c>
       <c r="G23" s="2">
@@ -1241,14 +1242,14 @@
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="11">
-        <v>5</v>
-      </c>
-      <c r="D24" s="11">
+      <c r="C24" s="9">
+        <v>5</v>
+      </c>
+      <c r="D24" s="9">
         <v>5</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="2">
+      <c r="F24" s="9">
         <v>5</v>
       </c>
       <c r="G24" s="2">
@@ -1272,14 +1273,14 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="9">
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="E25" s="9">
+        <v>5</v>
+      </c>
+      <c r="F25" s="9">
         <v>5</v>
       </c>
       <c r="H25" s="2">
@@ -1300,16 +1301,16 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="11">
-        <v>5</v>
-      </c>
-      <c r="D26" s="11">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="C26" s="9">
+        <v>5</v>
+      </c>
+      <c r="D26" s="9">
+        <v>5</v>
+      </c>
+      <c r="E26" s="9">
+        <v>5</v>
+      </c>
+      <c r="F26" s="9">
         <v>5</v>
       </c>
       <c r="G26" s="2">
@@ -1336,16 +1337,16 @@
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="11">
-        <v>5</v>
-      </c>
-      <c r="D27" s="11">
-        <v>5</v>
-      </c>
-      <c r="E27" s="2">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="C27" s="9">
+        <v>5</v>
+      </c>
+      <c r="D27" s="9">
+        <v>5</v>
+      </c>
+      <c r="E27" s="9">
+        <v>5</v>
+      </c>
+      <c r="F27" s="9">
         <v>5</v>
       </c>
       <c r="G27" s="2">
@@ -1372,16 +1373,16 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="11">
-        <v>5</v>
-      </c>
-      <c r="D28" s="11">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="C28" s="9">
+        <v>5</v>
+      </c>
+      <c r="D28" s="9">
+        <v>5</v>
+      </c>
+      <c r="E28" s="9">
+        <v>5</v>
+      </c>
+      <c r="F28" s="9">
         <v>5</v>
       </c>
       <c r="G28" s="2">
@@ -1408,12 +1409,12 @@
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="9">
         <v>5</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2">
+      <c r="F29" s="9">
         <v>5</v>
       </c>
       <c r="G29">
@@ -1456,10 +1457,10 @@
         <v>27</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="11">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2">
+      <c r="D31" s="9">
+        <v>5</v>
+      </c>
+      <c r="E31" s="9">
         <v>5</v>
       </c>
       <c r="K31" s="7">

</xml_diff>

<commit_message>
AutoCommit_4 декабря 2023 г. 14:28:39_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Каменецкий</t>
+  </si>
+  <si>
+    <t>Вырианты</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +194,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -262,7 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -276,9 +284,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -583,13 +599,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20:F29"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -647,6 +663,9 @@
       <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="K3" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
@@ -660,14 +679,14 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>5</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="9">
-        <v>5</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="8">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12">
         <v>5</v>
       </c>
       <c r="G5" s="2">
@@ -676,13 +695,7 @@
       <c r="H5" s="5">
         <v>5</v>
       </c>
-      <c r="K5">
-        <f>SUM(C5:I5)</f>
-        <v>25</v>
-      </c>
-      <c r="M5">
-        <v>4</v>
-      </c>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -691,16 +704,16 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9">
-        <v>5</v>
-      </c>
-      <c r="E6" s="9">
-        <v>5</v>
-      </c>
-      <c r="F6" s="9">
+      <c r="C6" s="8">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8">
         <v>5</v>
       </c>
       <c r="G6" s="2">
@@ -712,13 +725,7 @@
       <c r="I6" s="2">
         <v>5</v>
       </c>
-      <c r="K6" s="7">
-        <f t="shared" ref="K6:K31" si="0">SUM(C6:I6)</f>
-        <v>35</v>
-      </c>
-      <c r="M6">
-        <v>5</v>
-      </c>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -727,26 +734,20 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="9">
-        <v>5</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8">
         <v>5</v>
       </c>
       <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="K7" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M7">
-        <v>4</v>
-      </c>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -758,13 +759,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="K8" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -773,16 +768,16 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="9">
-        <v>5</v>
-      </c>
-      <c r="D9" s="9">
-        <v>5</v>
-      </c>
-      <c r="E9" s="9">
-        <v>5</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="C9" s="8">
+        <v>5</v>
+      </c>
+      <c r="D9" s="8">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8">
         <v>5</v>
       </c>
       <c r="G9" s="2">
@@ -794,12 +789,8 @@
       <c r="I9" s="2">
         <v>5</v>
       </c>
-      <c r="K9" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
+      <c r="K9" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -809,16 +800,16 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9">
-        <v>5</v>
-      </c>
-      <c r="D10" s="9">
-        <v>5</v>
-      </c>
-      <c r="E10" s="9">
-        <v>5</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>5</v>
+      </c>
+      <c r="F10" s="8">
         <v>5</v>
       </c>
       <c r="G10" s="2">
@@ -827,13 +818,7 @@
       <c r="H10" s="2">
         <v>5</v>
       </c>
-      <c r="K10" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M10">
-        <v>5</v>
-      </c>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -845,13 +830,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="K11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>2</v>
-      </c>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -860,16 +839,16 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9">
-        <v>5</v>
-      </c>
-      <c r="E12" s="9">
-        <v>5</v>
-      </c>
-      <c r="F12" s="9">
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="F12" s="8">
         <v>5</v>
       </c>
       <c r="G12" s="2">
@@ -882,34 +861,24 @@
         <v>5</v>
       </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="K12" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
         <v>9</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="H13" s="11">
-        <v>5</v>
-      </c>
-      <c r="K13" s="12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M13" s="12">
-        <v>2</v>
-      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="H13" s="10">
+        <v>5</v>
+      </c>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -918,16 +887,16 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="9">
-        <v>5</v>
-      </c>
-      <c r="D14" s="9">
-        <v>5</v>
-      </c>
-      <c r="E14" s="9">
-        <v>5</v>
-      </c>
-      <c r="F14" s="9">
+      <c r="C14" s="8">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8">
+        <v>5</v>
+      </c>
+      <c r="E14" s="8">
+        <v>5</v>
+      </c>
+      <c r="F14" s="8">
         <v>5</v>
       </c>
       <c r="G14" s="2">
@@ -936,13 +905,7 @@
       <c r="H14" s="2">
         <v>5</v>
       </c>
-      <c r="K14" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M14">
-        <v>5</v>
-      </c>
+      <c r="K14" s="16"/>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -951,16 +914,16 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="9">
-        <v>5</v>
-      </c>
-      <c r="D15" s="9">
-        <v>5</v>
-      </c>
-      <c r="E15" s="9">
-        <v>5</v>
-      </c>
-      <c r="F15" s="9">
+      <c r="C15" s="8">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8">
+        <v>5</v>
+      </c>
+      <c r="F15" s="8">
         <v>5</v>
       </c>
       <c r="G15" s="2">
@@ -973,12 +936,8 @@
         <v>5</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M15">
-        <v>5</v>
+      <c r="K15" s="16">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -988,16 +947,16 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="9">
-        <v>5</v>
-      </c>
-      <c r="D16" s="9">
-        <v>5</v>
-      </c>
-      <c r="E16" s="9">
-        <v>5</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="C16" s="8">
+        <v>5</v>
+      </c>
+      <c r="D16" s="8">
+        <v>5</v>
+      </c>
+      <c r="E16" s="8">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8">
         <v>5</v>
       </c>
       <c r="G16" s="2">
@@ -1009,31 +968,25 @@
       <c r="I16" s="2">
         <v>5</v>
       </c>
-      <c r="K16" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="9">
-        <v>5</v>
-      </c>
-      <c r="D17" s="9">
-        <v>5</v>
-      </c>
-      <c r="E17" s="9">
-        <v>5</v>
-      </c>
-      <c r="F17" s="9">
+      <c r="C17" s="8">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
+      <c r="F17" s="8">
         <v>5</v>
       </c>
       <c r="G17" s="2">
@@ -1045,15 +998,9 @@
       <c r="I17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1063,22 +1010,16 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="K18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>5</v>
       </c>
       <c r="D19" s="2"/>
@@ -1089,32 +1030,28 @@
       <c r="H19" s="2">
         <v>5</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="K19" s="7">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M19">
+      <c r="I19" s="7"/>
+      <c r="K19" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="9">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9">
-        <v>5</v>
-      </c>
-      <c r="E20" s="9">
-        <v>5</v>
-      </c>
-      <c r="F20" s="9">
+      <c r="C20" s="8">
+        <v>5</v>
+      </c>
+      <c r="D20" s="8">
+        <v>5</v>
+      </c>
+      <c r="E20" s="8">
+        <v>5</v>
+      </c>
+      <c r="F20" s="8">
         <v>5</v>
       </c>
       <c r="G20" s="2">
@@ -1126,29 +1063,23 @@
       <c r="I20" s="2">
         <v>5</v>
       </c>
-      <c r="K20" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="9">
-        <v>5</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="C21" s="8">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8">
         <v>5</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>5</v>
       </c>
       <c r="G21" s="2">
@@ -1158,31 +1089,25 @@
         <v>5</v>
       </c>
       <c r="I21" s="5"/>
-      <c r="K21" s="7">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="9">
-        <v>5</v>
-      </c>
-      <c r="D22" s="9">
-        <v>5</v>
-      </c>
-      <c r="E22" s="9">
-        <v>5</v>
-      </c>
-      <c r="F22" s="9">
+      <c r="C22" s="8">
+        <v>5</v>
+      </c>
+      <c r="D22" s="8">
+        <v>5</v>
+      </c>
+      <c r="E22" s="8">
+        <v>5</v>
+      </c>
+      <c r="F22" s="8">
         <v>5</v>
       </c>
       <c r="G22" s="2">
@@ -1194,31 +1119,25 @@
       <c r="I22" s="2">
         <v>5</v>
       </c>
-      <c r="K22" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="9">
-        <v>5</v>
-      </c>
-      <c r="D23" s="9">
-        <v>5</v>
-      </c>
-      <c r="E23" s="9">
-        <v>5</v>
-      </c>
-      <c r="F23" s="9">
+      <c r="C23" s="8">
+        <v>5</v>
+      </c>
+      <c r="D23" s="8">
+        <v>5</v>
+      </c>
+      <c r="E23" s="8">
+        <v>5</v>
+      </c>
+      <c r="F23" s="8">
         <v>5</v>
       </c>
       <c r="G23" s="2">
@@ -1227,29 +1146,23 @@
       <c r="H23" s="2">
         <v>5</v>
       </c>
-      <c r="K23" s="7">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="9">
-        <v>5</v>
-      </c>
-      <c r="D24" s="9">
+      <c r="C24" s="8">
+        <v>5</v>
+      </c>
+      <c r="D24" s="8">
         <v>5</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>5</v>
       </c>
       <c r="G24" s="2">
@@ -1258,59 +1171,49 @@
       <c r="I24" s="6">
         <v>5</v>
       </c>
-      <c r="K24" s="7">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>5</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="9">
-        <v>5</v>
-      </c>
-      <c r="F25" s="9">
+      <c r="E25" s="8">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8">
         <v>5</v>
       </c>
       <c r="H25" s="2">
         <v>5</v>
       </c>
-      <c r="K25" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="9">
-        <v>5</v>
-      </c>
-      <c r="D26" s="9">
-        <v>5</v>
-      </c>
-      <c r="E26" s="9">
-        <v>5</v>
-      </c>
-      <c r="F26" s="9">
+      <c r="C26" s="8">
+        <v>5</v>
+      </c>
+      <c r="D26" s="8">
+        <v>5</v>
+      </c>
+      <c r="E26" s="8">
+        <v>5</v>
+      </c>
+      <c r="F26" s="8">
         <v>5</v>
       </c>
       <c r="G26" s="2">
@@ -1322,31 +1225,25 @@
       <c r="I26" s="5">
         <v>5</v>
       </c>
-      <c r="K26" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="16"/>
+    </row>
+    <row r="27" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="9">
-        <v>5</v>
-      </c>
-      <c r="D27" s="9">
-        <v>5</v>
-      </c>
-      <c r="E27" s="9">
-        <v>5</v>
-      </c>
-      <c r="F27" s="9">
+      <c r="C27" s="8">
+        <v>5</v>
+      </c>
+      <c r="D27" s="8">
+        <v>5</v>
+      </c>
+      <c r="E27" s="8">
+        <v>5</v>
+      </c>
+      <c r="F27" s="8">
         <v>5</v>
       </c>
       <c r="G27" s="2">
@@ -1358,31 +1255,25 @@
       <c r="I27" s="2">
         <v>5</v>
       </c>
-      <c r="K27" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="9">
-        <v>5</v>
-      </c>
-      <c r="D28" s="9">
-        <v>5</v>
-      </c>
-      <c r="E28" s="9">
-        <v>5</v>
-      </c>
-      <c r="F28" s="9">
+      <c r="C28" s="8">
+        <v>5</v>
+      </c>
+      <c r="D28" s="8">
+        <v>5</v>
+      </c>
+      <c r="E28" s="8">
+        <v>5</v>
+      </c>
+      <c r="F28" s="8">
         <v>5</v>
       </c>
       <c r="G28" s="2">
@@ -1394,27 +1285,21 @@
       <c r="I28" s="2">
         <v>5</v>
       </c>
-      <c r="K28" s="7">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>5</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="9">
+      <c r="F29" s="8">
         <v>5</v>
       </c>
       <c r="G29">
@@ -1423,15 +1308,11 @@
       <c r="H29" s="2">
         <v>5</v>
       </c>
-      <c r="K29" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1441,15 +1322,9 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="K30" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="K30" s="16"/>
+    </row>
+    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1457,21 +1332,15 @@
         <v>27</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="9">
-        <v>5</v>
-      </c>
-      <c r="E31" s="9">
-        <v>5</v>
-      </c>
-      <c r="K31" s="7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="8">
+        <v>5</v>
+      </c>
+      <c r="E31" s="8">
+        <v>5</v>
+      </c>
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:11" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>1</v>
       </c>
@@ -1481,8 +1350,9 @@
       <c r="E32" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K32" s="16"/>
+    </row>
+    <row r="33" spans="2:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1504,25 +1374,55 @@
       <c r="H33" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="2:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="16"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="16"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="16"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="16"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="16"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="16"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="16"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="16"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="16"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K5:K31">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M5:M31">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>

<commit_message>
AutoCommit_4 декабря 2023 г. 14:39:22_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -285,8 +285,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -295,6 +293,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -602,10 +602,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -616,29 +616,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -663,7 +663,7 @@
       <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
@@ -695,7 +695,7 @@
       <c r="H5" s="5">
         <v>5</v>
       </c>
-      <c r="K5" s="16"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -725,7 +725,7 @@
       <c r="I6" s="2">
         <v>5</v>
       </c>
-      <c r="K6" s="16"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -747,7 +747,7 @@
       <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="K7" s="16"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -759,7 +759,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="K8" s="16"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -789,7 +789,10 @@
       <c r="I9" s="2">
         <v>5</v>
       </c>
-      <c r="K9" s="17">
+      <c r="J9" s="5">
+        <v>5</v>
+      </c>
+      <c r="K9" s="15">
         <v>1</v>
       </c>
     </row>
@@ -818,7 +821,7 @@
       <c r="H10" s="2">
         <v>5</v>
       </c>
-      <c r="K10" s="16"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -830,7 +833,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="K11" s="16"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -861,7 +864,7 @@
         <v>5</v>
       </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="16">
+      <c r="K12" s="14">
         <v>2</v>
       </c>
     </row>
@@ -878,7 +881,7 @@
       <c r="H13" s="10">
         <v>5</v>
       </c>
-      <c r="K13" s="18"/>
+      <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -905,7 +908,7 @@
       <c r="H14" s="2">
         <v>5</v>
       </c>
-      <c r="K14" s="16"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -935,8 +938,10 @@
       <c r="I15" s="5">
         <v>5</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="16">
+      <c r="J15" s="2">
+        <v>5</v>
+      </c>
+      <c r="K15" s="14">
         <v>2</v>
       </c>
     </row>
@@ -968,7 +973,7 @@
       <c r="I16" s="2">
         <v>5</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -998,7 +1003,7 @@
       <c r="I17" s="2">
         <v>5</v>
       </c>
-      <c r="K17" s="16"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -1010,7 +1015,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="K18" s="16"/>
+      <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -1031,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="K19" s="16">
+      <c r="K19" s="14">
         <v>3</v>
       </c>
     </row>
@@ -1063,7 +1068,7 @@
       <c r="I20" s="2">
         <v>5</v>
       </c>
-      <c r="K20" s="16"/>
+      <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -1089,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="I21" s="5"/>
-      <c r="K21" s="16"/>
+      <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1119,7 +1124,7 @@
       <c r="I22" s="2">
         <v>5</v>
       </c>
-      <c r="K22" s="16"/>
+      <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -1146,7 +1151,7 @@
       <c r="H23" s="2">
         <v>5</v>
       </c>
-      <c r="K23" s="16"/>
+      <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1171,7 +1176,7 @@
       <c r="I24" s="6">
         <v>5</v>
       </c>
-      <c r="K24" s="16">
+      <c r="K24" s="14">
         <v>2</v>
       </c>
     </row>
@@ -1195,7 +1200,7 @@
       <c r="H25" s="2">
         <v>5</v>
       </c>
-      <c r="K25" s="16"/>
+      <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -1225,7 +1230,7 @@
       <c r="I26" s="5">
         <v>5</v>
       </c>
-      <c r="K26" s="16"/>
+      <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -1255,7 +1260,7 @@
       <c r="I27" s="2">
         <v>5</v>
       </c>
-      <c r="K27" s="16"/>
+      <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -1285,7 +1290,7 @@
       <c r="I28" s="2">
         <v>5</v>
       </c>
-      <c r="K28" s="16"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1308,7 +1313,7 @@
       <c r="H29" s="2">
         <v>5</v>
       </c>
-      <c r="K29" s="16">
+      <c r="K29" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1322,7 +1327,9 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="K30" s="16"/>
+      <c r="K30" s="14">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1338,7 +1345,9 @@
       <c r="E31" s="8">
         <v>5</v>
       </c>
-      <c r="K31" s="16"/>
+      <c r="K31" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
@@ -1350,7 +1359,7 @@
       <c r="E32" s="3">
         <v>1</v>
       </c>
-      <c r="K32" s="16"/>
+      <c r="K32" s="14"/>
     </row>
     <row r="33" spans="2:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
@@ -1374,49 +1383,49 @@
       <c r="H33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K33" s="16"/>
+      <c r="K33" s="14"/>
     </row>
     <row r="34" spans="2:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K34" s="16"/>
+      <c r="K34" s="14"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K35" s="16"/>
+      <c r="K35" s="14"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K36" s="16"/>
+      <c r="K36" s="14"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K37" s="16"/>
+      <c r="K37" s="14"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K38" s="16"/>
+      <c r="K38" s="14"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K39" s="16"/>
+      <c r="K39" s="14"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K40" s="16"/>
+      <c r="K40" s="14"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K41" s="16"/>
+      <c r="K41" s="14"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K42" s="16"/>
+      <c r="K42" s="14"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K43" s="16"/>
+      <c r="K43" s="14"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K44" s="16"/>
+      <c r="K44" s="14"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K45" s="16"/>
+      <c r="K45" s="14"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K46" s="16"/>
+      <c r="K46" s="14"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K47" s="16"/>
+      <c r="K47" s="14"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_4 декабря 2023 г. 15:14:22_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -602,10 +602,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1302,8 +1302,12 @@
       <c r="C29" s="8">
         <v>5</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
       <c r="F29" s="8">
         <v>5</v>
       </c>
@@ -1311,6 +1315,12 @@
         <v>5</v>
       </c>
       <c r="H29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29" s="6">
+        <v>5</v>
+      </c>
+      <c r="J29" s="6">
         <v>5</v>
       </c>
       <c r="K29" s="14">

</xml_diff>

<commit_message>
AutoCommit_7 декабря 2023 г. 11:26:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -702,7 +702,7 @@
       </c>
       <c r="N4" s="17">
         <f t="shared" ref="N4:P4" si="0">SUM(N5:N35)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O4" s="17">
         <f t="shared" si="0"/>
@@ -1208,14 +1208,16 @@
       <c r="I16" s="2">
         <v>5</v>
       </c>
-      <c r="L16" s="14"/>
+      <c r="L16" s="14">
+        <v>2</v>
+      </c>
       <c r="M16" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N16" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="17">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 14:03:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -911,6 +911,9 @@
       <c r="J9" s="5">
         <v>5</v>
       </c>
+      <c r="K9" s="5">
+        <v>5</v>
+      </c>
       <c r="L9" s="15">
         <v>1</v>
       </c>
@@ -1032,7 +1035,12 @@
       <c r="I12" s="5">
         <v>5</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="5">
+        <v>5</v>
+      </c>
       <c r="L12" s="14">
         <v>2</v>
       </c>
@@ -1206,6 +1214,12 @@
         <v>5</v>
       </c>
       <c r="I16" s="2">
+        <v>5</v>
+      </c>
+      <c r="J16" s="5">
+        <v>5</v>
+      </c>
+      <c r="K16" s="5">
         <v>5</v>
       </c>
       <c r="L16" s="14">
@@ -1374,6 +1388,12 @@
       <c r="I20" s="2">
         <v>5</v>
       </c>
+      <c r="J20" s="7">
+        <v>5</v>
+      </c>
+      <c r="K20" s="7">
+        <v>5</v>
+      </c>
       <c r="L20" s="14">
         <v>4</v>
       </c>
@@ -1471,6 +1491,9 @@
       <c r="J22" s="5">
         <v>5</v>
       </c>
+      <c r="K22" s="5">
+        <v>5</v>
+      </c>
       <c r="L22" s="14">
         <v>3</v>
       </c>
@@ -1565,6 +1588,9 @@
       <c r="J24" s="6">
         <v>5</v>
       </c>
+      <c r="K24" s="6">
+        <v>5</v>
+      </c>
       <c r="L24" s="14">
         <v>2</v>
       </c>
@@ -1654,6 +1680,9 @@
       <c r="J26" s="5">
         <v>5</v>
       </c>
+      <c r="K26" s="5">
+        <v>5</v>
+      </c>
       <c r="L26" s="14">
         <v>4</v>
       </c>
@@ -1754,6 +1783,9 @@
         <v>5</v>
       </c>
       <c r="J28" s="5">
+        <v>5</v>
+      </c>
+      <c r="K28" s="5">
         <v>5</v>
       </c>
       <c r="L28" s="14">

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 14:36:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -612,7 +612,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomRight" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -792,6 +792,9 @@
       <c r="J6" s="5">
         <v>5</v>
       </c>
+      <c r="K6" s="5">
+        <v>5</v>
+      </c>
       <c r="L6" s="14">
         <v>3</v>
       </c>
@@ -933,6 +936,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1060,6 +1066,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="R12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:23" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
@@ -1271,6 +1280,9 @@
         <v>5</v>
       </c>
       <c r="J17" s="5">
+        <v>5</v>
+      </c>
+      <c r="K17" s="5">
         <v>5</v>
       </c>
       <c r="L17" s="14">
@@ -1734,6 +1746,9 @@
       <c r="J27" s="5">
         <v>5</v>
       </c>
+      <c r="K27" s="5">
+        <v>5</v>
+      </c>
       <c r="L27" s="14">
         <v>4</v>
       </c>
@@ -1837,6 +1852,9 @@
         <v>5</v>
       </c>
       <c r="J29" s="6">
+        <v>5</v>
+      </c>
+      <c r="K29" s="7">
         <v>5</v>
       </c>
       <c r="L29" s="14">

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 15:08:55_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R9" sqref="R9"/>
+      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -814,6 +814,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="R6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -1250,8 +1253,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1333,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1372,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -1426,7 +1432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -1569,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1622,8 +1628,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1715,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1877,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1907,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1941,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_11 декабря 2023 г. 16:05:59_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="K7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1531,6 +1531,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="R22">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -1777,6 +1780,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="R27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -1830,6 +1836,9 @@
       <c r="P28" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
+      </c>
+      <c r="R28">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 8:52:42_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -609,10 +609,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1199,6 +1199,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="R15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1725,6 +1728,9 @@
       <c r="P26" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
+      </c>
+      <c r="R26">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 9:35:37_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -300,6 +300,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -609,10 +612,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
+      <selection pane="bottomRight" activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -623,29 +626,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
+      <c r="C1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -741,6 +744,12 @@
       <c r="I5" s="5">
         <v>5</v>
       </c>
+      <c r="J5" s="5">
+        <v>5</v>
+      </c>
+      <c r="K5" s="5">
+        <v>5</v>
+      </c>
       <c r="L5" s="14">
         <v>3</v>
       </c>
@@ -1129,6 +1138,15 @@
       <c r="H14" s="2">
         <v>5</v>
       </c>
+      <c r="I14" s="18">
+        <v>5</v>
+      </c>
+      <c r="J14" s="18">
+        <v>5</v>
+      </c>
+      <c r="K14" s="18">
+        <v>5</v>
+      </c>
       <c r="L14" s="14">
         <v>2</v>
       </c>
@@ -1147,6 +1165,9 @@
       <c r="P14" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="R14">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1312,6 +1333,9 @@
       <c r="P17" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="R17">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1434,6 +1458,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -1448,7 +1475,9 @@
       <c r="D21" s="8">
         <v>5</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
       <c r="F21" s="8">
         <v>5</v>
       </c>
@@ -1459,6 +1488,9 @@
         <v>5</v>
       </c>
       <c r="I21" s="5">
+        <v>5</v>
+      </c>
+      <c r="J21" s="7">
         <v>5</v>
       </c>
       <c r="L21" s="14">
@@ -1563,6 +1595,12 @@
       <c r="H23" s="2">
         <v>5</v>
       </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>5</v>
+      </c>
       <c r="L23" s="14"/>
       <c r="M23" s="17">
         <f t="shared" si="2"/>
@@ -1899,6 +1937,9 @@
       <c r="P29" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="R29">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 10:00:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -615,7 +615,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S29" sqref="S29"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
       </c>
       <c r="P4" s="17">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -768,6 +768,9 @@
       <c r="P5" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -874,10 +877,27 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="L8" s="14"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7">
+        <v>5</v>
+      </c>
+      <c r="L8" s="14">
+        <v>4</v>
+      </c>
       <c r="M8" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -892,7 +912,7 @@
       </c>
       <c r="P8" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1376,15 +1396,27 @@
       <c r="C19" s="8">
         <v>5</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="15">
+        <v>5</v>
+      </c>
       <c r="G19" s="2">
         <v>5</v>
       </c>
       <c r="H19" s="2">
         <v>5</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="7">
+        <v>5</v>
+      </c>
+      <c r="J19" s="7">
+        <v>5</v>
+      </c>
       <c r="L19" s="14">
         <v>3</v>
       </c>
@@ -1512,6 +1544,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="R21">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1595,6 +1630,9 @@
       <c r="H23" s="2">
         <v>5</v>
       </c>
+      <c r="I23" s="7">
+        <v>5</v>
+      </c>
       <c r="J23">
         <v>5</v>
       </c>
@@ -1617,6 +1655,9 @@
       <c r="P23" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="R23">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1949,9 +1990,27 @@
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="C30" s="2">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="18">
+        <v>5</v>
+      </c>
+      <c r="G30" s="14">
+        <v>5</v>
+      </c>
+      <c r="H30" s="14">
+        <v>5</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
       <c r="L30" s="14">
         <v>4</v>
       </c>
@@ -1979,11 +2038,19 @@
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2">
+        <v>5</v>
+      </c>
       <c r="D31" s="8">
         <v>5</v>
       </c>
       <c r="E31" s="8">
+        <v>5</v>
+      </c>
+      <c r="G31" s="7">
+        <v>5</v>
+      </c>
+      <c r="H31" s="7">
         <v>5</v>
       </c>
       <c r="L31" s="14">

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 16:55:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -615,7 +615,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -914,6 +914,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -2101,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -2148,47 +2151,50 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L34" s="14"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K35" s="14"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K36" s="14"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K37" s="14"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K38" s="14"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K39" s="14"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K40" s="14"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K41" s="14"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K42" s="14"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K43" s="14"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K44" s="14"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K45" s="14"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K46" s="14"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K47" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 17:24:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -615,7 +615,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
+      <selection pane="bottomRight" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1439,6 +1439,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="R19">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 18:24:56_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -612,10 +612,10 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R19" sqref="R19"/>
+      <selection pane="bottomRight" activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2036,6 +2036,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="R30">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 22:55:29_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Гарас Кристина</t>
-  </si>
-  <si>
-    <t>Голубов Алексей</t>
   </si>
   <si>
     <t>Горинова Полина</t>
@@ -145,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -168,23 +165,8 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,12 +176,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -283,24 +259,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -609,13 +577,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W47"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S30" sqref="S30"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -626,61 +594,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
+      <c r="C1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>37</v>
+      <c r="L3" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -700,19 +668,19 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="M4">
-        <f>SUM(M5:M35)</f>
+        <f>SUM(M5:M34)</f>
         <v>6</v>
       </c>
-      <c r="N4" s="17">
-        <f t="shared" ref="N4:P4" si="0">SUM(N5:N35)</f>
+      <c r="N4" s="13">
+        <f>SUM(N5:N34)</f>
         <v>6</v>
       </c>
-      <c r="O4" s="17">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="P4" s="17">
-        <f t="shared" si="0"/>
+      <c r="O4" s="13">
+        <f>SUM(O5:O34)</f>
+        <v>5</v>
+      </c>
+      <c r="P4" s="13">
+        <f>SUM(P5:P34)</f>
         <v>6</v>
       </c>
     </row>
@@ -732,7 +700,7 @@
       <c r="E5" s="8">
         <v>5</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="9">
         <v>5</v>
       </c>
       <c r="G5" s="2">
@@ -750,23 +718,23 @@
       <c r="K5" s="5">
         <v>5</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="11">
         <v>3</v>
       </c>
       <c r="M5">
         <f>IF($L5=M$3,1,0)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="17">
-        <f t="shared" ref="N5:P20" si="1">IF($L5=N$3,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P5" s="17">
-        <f t="shared" si="1"/>
+      <c r="N5" s="13">
+        <f t="shared" ref="N5:P19" si="0">IF($L5=N$3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P5" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R5">
@@ -807,23 +775,23 @@
       <c r="K6" s="5">
         <v>5</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="11">
         <v>3</v>
       </c>
-      <c r="M6" s="17">
-        <f t="shared" ref="M6:P33" si="2">IF($L6=M$3,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P6" s="17">
-        <f t="shared" si="1"/>
+      <c r="M6" s="13">
+        <f t="shared" ref="M6:P32" si="1">IF($L6=M$3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P6" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R6">
@@ -850,23 +818,23 @@
       <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="L7" s="14">
-        <v>1</v>
-      </c>
-      <c r="M7" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N7" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="17">
-        <f t="shared" si="1"/>
+      <c r="L7" s="11">
+        <v>1</v>
+      </c>
+      <c r="M7" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -895,23 +863,23 @@
       <c r="H8" s="7">
         <v>5</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="11">
         <v>4</v>
       </c>
-      <c r="M8" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="17">
-        <f t="shared" si="1"/>
+      <c r="M8" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="13">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R8">
@@ -952,23 +920,23 @@
       <c r="K9" s="5">
         <v>5</v>
       </c>
-      <c r="L9" s="15">
-        <v>1</v>
-      </c>
-      <c r="M9" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N9" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="17">
-        <f t="shared" si="1"/>
+      <c r="L9" s="12">
+        <v>1</v>
+      </c>
+      <c r="M9" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R9">
@@ -1000,23 +968,23 @@
       <c r="H10" s="2">
         <v>5</v>
       </c>
-      <c r="L10" s="14">
-        <v>1</v>
-      </c>
-      <c r="M10" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N10" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="17">
-        <f t="shared" si="1"/>
+      <c r="L10" s="11">
+        <v>1</v>
+      </c>
+      <c r="M10" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1030,21 +998,21 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="17">
-        <f t="shared" si="1"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1082,63 +1050,89 @@
       <c r="K12" s="5">
         <v>5</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="11">
         <v>2</v>
       </c>
-      <c r="M12" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="17">
-        <f t="shared" si="1"/>
+      <c r="M12" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="H13" s="10">
-        <v>5</v>
-      </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C13" s="8">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="8">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="I13" s="14">
+        <v>5</v>
+      </c>
+      <c r="J13" s="14">
+        <v>5</v>
+      </c>
+      <c r="K13" s="14">
+        <v>5</v>
+      </c>
+      <c r="L13" s="11">
+        <v>2</v>
+      </c>
+      <c r="M13" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -1161,32 +1155,29 @@
       <c r="H14" s="2">
         <v>5</v>
       </c>
-      <c r="I14" s="18">
-        <v>5</v>
-      </c>
-      <c r="J14" s="18">
-        <v>5</v>
-      </c>
-      <c r="K14" s="18">
-        <v>5</v>
-      </c>
-      <c r="L14" s="14">
+      <c r="I14" s="5">
+        <v>5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5</v>
+      </c>
+      <c r="L14" s="11">
         <v>2</v>
       </c>
-      <c r="M14" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="17">
-        <f t="shared" si="1"/>
+      <c r="M14" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R14">
@@ -1195,7 +1186,7 @@
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -1218,29 +1209,32 @@
       <c r="H15" s="2">
         <v>5</v>
       </c>
-      <c r="I15" s="5">
-        <v>5</v>
-      </c>
-      <c r="J15" s="2">
-        <v>5</v>
-      </c>
-      <c r="L15" s="14">
+      <c r="I15" s="2">
+        <v>5</v>
+      </c>
+      <c r="J15" s="5">
+        <v>5</v>
+      </c>
+      <c r="K15" s="5">
+        <v>5</v>
+      </c>
+      <c r="L15" s="11">
         <v>2</v>
       </c>
-      <c r="M15" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O15" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="17">
-        <f t="shared" si="1"/>
+      <c r="M15" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R15">
@@ -1249,7 +1243,7 @@
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -1281,23 +1275,23 @@
       <c r="K16" s="5">
         <v>5</v>
       </c>
-      <c r="L16" s="14">
-        <v>2</v>
-      </c>
-      <c r="M16" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="17">
-        <f t="shared" si="1"/>
+      <c r="L16" s="11">
+        <v>1</v>
+      </c>
+      <c r="M16" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R16">
@@ -1306,92 +1300,89 @@
     </row>
     <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="8">
-        <v>5</v>
-      </c>
-      <c r="D17" s="8">
-        <v>5</v>
-      </c>
-      <c r="E17" s="8">
-        <v>5</v>
-      </c>
-      <c r="F17" s="8">
-        <v>5</v>
-      </c>
-      <c r="G17" s="2">
-        <v>5</v>
-      </c>
-      <c r="H17" s="2">
-        <v>5</v>
-      </c>
-      <c r="I17" s="2">
-        <v>5</v>
-      </c>
-      <c r="J17" s="5">
-        <v>5</v>
-      </c>
-      <c r="K17" s="5">
-        <v>5</v>
-      </c>
-      <c r="L17" s="14">
-        <v>1</v>
-      </c>
-      <c r="M17" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N17" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>5</v>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C18" s="8">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" s="7">
+        <v>5</v>
+      </c>
+      <c r="J18" s="7">
+        <v>5</v>
+      </c>
+      <c r="L18" s="11">
+        <v>3</v>
+      </c>
+      <c r="M18" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P18" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
@@ -1399,13 +1390,13 @@
       <c r="C19" s="8">
         <v>5</v>
       </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="15">
+      <c r="D19" s="8">
+        <v>5</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5</v>
+      </c>
+      <c r="F19" s="8">
         <v>5</v>
       </c>
       <c r="G19" s="2">
@@ -1414,38 +1405,41 @@
       <c r="H19" s="2">
         <v>5</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="2">
         <v>5</v>
       </c>
       <c r="J19" s="7">
         <v>5</v>
       </c>
-      <c r="L19" s="14">
-        <v>3</v>
-      </c>
-      <c r="M19" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P19" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="K19" s="7">
+        <v>5</v>
+      </c>
+      <c r="L19" s="11">
+        <v>4</v>
+      </c>
+      <c r="M19" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
@@ -1456,7 +1450,7 @@
       <c r="D20" s="8">
         <v>5</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="2">
         <v>5</v>
       </c>
       <c r="F20" s="8">
@@ -1468,33 +1462,30 @@
       <c r="H20" s="2">
         <v>5</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="5">
         <v>5</v>
       </c>
       <c r="J20" s="7">
         <v>5</v>
       </c>
-      <c r="K20" s="7">
-        <v>5</v>
-      </c>
-      <c r="L20" s="14">
-        <v>4</v>
-      </c>
-      <c r="M20" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="17">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="L20" s="11">
+        <v>2</v>
+      </c>
+      <c r="M20" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="R20">
         <v>5</v>
@@ -1502,7 +1493,7 @@
     </row>
     <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
@@ -1513,7 +1504,7 @@
       <c r="D21" s="8">
         <v>5</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="8">
         <v>5</v>
       </c>
       <c r="F21" s="8">
@@ -1525,29 +1516,32 @@
       <c r="H21" s="2">
         <v>5</v>
       </c>
-      <c r="I21" s="5">
-        <v>5</v>
-      </c>
-      <c r="J21" s="7">
-        <v>5</v>
-      </c>
-      <c r="L21" s="14">
-        <v>2</v>
-      </c>
-      <c r="M21" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O21" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="17">
-        <f t="shared" si="2"/>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
+      <c r="J21" s="5">
+        <v>5</v>
+      </c>
+      <c r="K21" s="5">
+        <v>5</v>
+      </c>
+      <c r="L21" s="11">
+        <v>3</v>
+      </c>
+      <c r="M21" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="13">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R21">
@@ -1556,7 +1550,7 @@
     </row>
     <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
@@ -1579,32 +1573,30 @@
       <c r="H22" s="2">
         <v>5</v>
       </c>
-      <c r="I22" s="2">
-        <v>5</v>
-      </c>
-      <c r="J22" s="5">
-        <v>5</v>
-      </c>
-      <c r="K22" s="5">
-        <v>5</v>
-      </c>
-      <c r="L22" s="14">
-        <v>3</v>
-      </c>
-      <c r="M22" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P22" s="17">
-        <f t="shared" si="2"/>
+      <c r="I22" s="7">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22" s="11"/>
+      <c r="M22" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="13">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R22">
@@ -1613,7 +1605,7 @@
     </row>
     <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>19</v>
@@ -1624,7 +1616,7 @@
       <c r="D23" s="8">
         <v>5</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="2">
         <v>5</v>
       </c>
       <c r="F23" s="8">
@@ -1633,33 +1625,35 @@
       <c r="G23" s="2">
         <v>5</v>
       </c>
-      <c r="H23" s="2">
-        <v>5</v>
-      </c>
-      <c r="I23" s="7">
-        <v>5</v>
-      </c>
-      <c r="J23">
-        <v>5</v>
-      </c>
-      <c r="K23">
-        <v>5</v>
-      </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="17">
-        <f t="shared" si="2"/>
+      <c r="H23" s="5">
+        <v>5</v>
+      </c>
+      <c r="I23" s="6">
+        <v>5</v>
+      </c>
+      <c r="J23" s="6">
+        <v>5</v>
+      </c>
+      <c r="K23" s="6">
+        <v>5</v>
+      </c>
+      <c r="L23" s="11">
+        <v>2</v>
+      </c>
+      <c r="M23" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O23" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="13">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R23">
@@ -1668,7 +1662,7 @@
     </row>
     <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -1676,56 +1670,37 @@
       <c r="C24" s="8">
         <v>5</v>
       </c>
-      <c r="D24" s="8">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="2"/>
+      <c r="E24" s="8">
         <v>5</v>
       </c>
       <c r="F24" s="8">
         <v>5</v>
       </c>
-      <c r="G24" s="2">
-        <v>5</v>
-      </c>
-      <c r="H24" s="5">
-        <v>5</v>
-      </c>
-      <c r="I24" s="6">
-        <v>5</v>
-      </c>
-      <c r="J24" s="6">
-        <v>5</v>
-      </c>
-      <c r="K24" s="6">
-        <v>5</v>
-      </c>
-      <c r="L24" s="14">
-        <v>2</v>
-      </c>
-      <c r="M24" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O24" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>5</v>
+      <c r="H24" s="2">
+        <v>5</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -1733,37 +1708,56 @@
       <c r="C25" s="8">
         <v>5</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="8">
+        <v>5</v>
+      </c>
       <c r="E25" s="8">
         <v>5</v>
       </c>
       <c r="F25" s="8">
         <v>5</v>
       </c>
+      <c r="G25" s="2">
+        <v>5</v>
+      </c>
       <c r="H25" s="2">
         <v>5</v>
       </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="I25" s="5">
+        <v>5</v>
+      </c>
+      <c r="J25" s="5">
+        <v>5</v>
+      </c>
+      <c r="K25" s="5">
+        <v>5</v>
+      </c>
+      <c r="L25" s="11">
+        <v>4</v>
+      </c>
+      <c r="M25" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>22</v>
@@ -1786,7 +1780,7 @@
       <c r="H26" s="2">
         <v>5</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="2">
         <v>5</v>
       </c>
       <c r="J26" s="5">
@@ -1795,23 +1789,23 @@
       <c r="K26" s="5">
         <v>5</v>
       </c>
-      <c r="L26" s="14">
+      <c r="L26" s="11">
         <v>4</v>
       </c>
-      <c r="M26" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="17">
-        <f t="shared" si="2"/>
+      <c r="M26" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="13">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R26">
@@ -1820,7 +1814,7 @@
     </row>
     <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
@@ -1852,23 +1846,23 @@
       <c r="K27" s="5">
         <v>5</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="11">
         <v>4</v>
       </c>
-      <c r="M27" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="17">
-        <f t="shared" si="2"/>
+      <c r="M27" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="13">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R27">
@@ -1877,7 +1871,7 @@
     </row>
     <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>24</v>
@@ -1885,48 +1879,48 @@
       <c r="C28" s="8">
         <v>5</v>
       </c>
-      <c r="D28" s="8">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8">
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2">
         <v>5</v>
       </c>
       <c r="F28" s="8">
         <v>5</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28">
         <v>5</v>
       </c>
       <c r="H28" s="2">
         <v>5</v>
       </c>
-      <c r="I28" s="2">
-        <v>5</v>
-      </c>
-      <c r="J28" s="5">
-        <v>5</v>
-      </c>
-      <c r="K28" s="5">
-        <v>5</v>
-      </c>
-      <c r="L28" s="14">
-        <v>4</v>
-      </c>
-      <c r="M28" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
+      <c r="I28" s="6">
+        <v>5</v>
+      </c>
+      <c r="J28" s="6">
+        <v>5</v>
+      </c>
+      <c r="K28" s="7">
+        <v>5</v>
+      </c>
+      <c r="L28" s="11">
+        <v>1</v>
+      </c>
+      <c r="M28" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N28" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="R28">
         <v>5</v>
@@ -1934,12 +1928,12 @@
     </row>
     <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="2">
         <v>5</v>
       </c>
       <c r="D29" s="2">
@@ -1948,42 +1942,36 @@
       <c r="E29" s="2">
         <v>5</v>
       </c>
-      <c r="F29" s="8">
-        <v>5</v>
-      </c>
-      <c r="G29">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2">
-        <v>5</v>
-      </c>
-      <c r="I29" s="6">
-        <v>5</v>
-      </c>
-      <c r="J29" s="6">
-        <v>5</v>
-      </c>
-      <c r="K29" s="7">
-        <v>5</v>
-      </c>
-      <c r="L29" s="14">
-        <v>1</v>
-      </c>
-      <c r="M29" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N29" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="F29" s="14">
+        <v>5</v>
+      </c>
+      <c r="G29" s="11">
+        <v>5</v>
+      </c>
+      <c r="H29" s="11">
+        <v>5</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11">
+        <v>4</v>
+      </c>
+      <c r="M29" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R29">
         <v>5</v>
@@ -1991,7 +1979,7 @@
     </row>
     <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>26</v>
@@ -1999,209 +1987,158 @@
       <c r="C30" s="2">
         <v>5</v>
       </c>
-      <c r="D30" s="2">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2">
-        <v>5</v>
-      </c>
-      <c r="F30" s="18">
-        <v>5</v>
-      </c>
-      <c r="G30" s="14">
-        <v>5</v>
-      </c>
-      <c r="H30" s="14">
-        <v>5</v>
-      </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14">
-        <v>4</v>
-      </c>
-      <c r="M30" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="R30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>27</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="2">
-        <v>5</v>
-      </c>
-      <c r="D31" s="8">
-        <v>5</v>
-      </c>
-      <c r="E31" s="8">
-        <v>5</v>
-      </c>
-      <c r="G31" s="7">
-        <v>5</v>
-      </c>
-      <c r="H31" s="7">
-        <v>5</v>
-      </c>
-      <c r="L31" s="14">
+      <c r="D30" s="8">
+        <v>5</v>
+      </c>
+      <c r="E30" s="8">
+        <v>5</v>
+      </c>
+      <c r="G30" s="7">
+        <v>5</v>
+      </c>
+      <c r="H30" s="7">
+        <v>5</v>
+      </c>
+      <c r="L30" s="11">
         <v>3</v>
       </c>
-      <c r="M31" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P31" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="3">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1</v>
-      </c>
-      <c r="L32" s="14"/>
-      <c r="M32" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O32" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P32" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I33">
-        <v>5</v>
-      </c>
-      <c r="J33">
-        <v>5</v>
-      </c>
-      <c r="L33" s="14">
-        <v>1</v>
-      </c>
-      <c r="M33" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N33" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O33" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P33" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:18" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L34" s="14"/>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K47" s="14"/>
+      <c r="M30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P30" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="L31" s="11"/>
+      <c r="M31" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="L32" s="11">
+        <v>1</v>
+      </c>
+      <c r="M32" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N32" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="11"/>
+    </row>
+    <row r="34" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K34" s="11"/>
+    </row>
+    <row r="35" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K35" s="11"/>
+    </row>
+    <row r="36" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="11"/>
+    </row>
+    <row r="37" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K37" s="11"/>
+    </row>
+    <row r="38" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K38" s="11"/>
+    </row>
+    <row r="39" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K39" s="11"/>
+    </row>
+    <row r="40" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K40" s="11"/>
+    </row>
+    <row r="41" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K41" s="11"/>
+    </row>
+    <row r="42" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K42" s="11"/>
+    </row>
+    <row r="43" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K43" s="11"/>
+    </row>
+    <row r="44" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K44" s="11"/>
+    </row>
+    <row r="45" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K45" s="11"/>
+    </row>
+    <row r="46" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K46" s="11"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_13 декабря 2023 г. 9:29:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_ДисМат_.xlsx
+++ b/2ИСИП-322_ДисМат_.xlsx
@@ -580,10 +580,10 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>